<commit_message>
-more values to calibrations
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Mass</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>StartClimb</t>
+  </si>
+  <si>
+    <t>3 significant digits</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D6"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +377,11 @@
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
@@ -412,6 +420,42 @@
       <c r="B6">
         <f>B5+4.575</f>
         <v>13.07</v>
+      </c>
+      <c r="C6">
+        <v>-0.81799999999999995</v>
+      </c>
+      <c r="D6">
+        <v>-0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>B6+4.54</f>
+        <v>17.61</v>
+      </c>
+      <c r="C7">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="D7">
+        <v>-1.161</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>B7+4.58</f>
+        <v>22.189999999999998</v>
+      </c>
+      <c r="C8">
+        <v>-1.4379999999999999</v>
+      </c>
+      <c r="D8">
+        <v>-1.526</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>B8+4.635</f>
+        <v>26.824999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Enchancing code -Adding new excel results
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="1st run" sheetId="3" r:id="rId3"/>
     <sheet name="2nd run" sheetId="4" r:id="rId4"/>
+    <sheet name="3rd run" sheetId="5" r:id="rId5"/>
+    <sheet name="Template" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="22">
   <si>
     <t>Mass</t>
   </si>
@@ -70,12 +71,27 @@
   <si>
     <t>Stiffness:70</t>
   </si>
+  <si>
+    <t>Stiffness</t>
+  </si>
+  <si>
+    <t>1/10 ratio</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>PULLEY BREAKS, Re-Did Pulley</t>
+  </si>
+  <si>
+    <t>Re-done</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +99,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +202,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -350,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92805888"/>
-        <c:axId val="92806464"/>
+        <c:axId val="40112064"/>
+        <c:axId val="40112640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92805888"/>
+        <c:axId val="40112064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,12 +401,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92806464"/>
+        <c:crossAx val="40112640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92806464"/>
+        <c:axId val="40112640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +417,153 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92805888"/>
+        <c:crossAx val="40112064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3rd run'!$C$36:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3rd run'!$D$36:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.277907407407412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.774528973201786</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.457259050696365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8318482119283015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7746968597252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="89113728"/>
+        <c:axId val="89112576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="89113728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89112576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="89112576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89113728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -416,6 +599,41 @@
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1060,18 +1278,18 @@
         <v>19.75</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F12" si="0">E5-D5</f>
+        <f t="shared" ref="F5:F6" si="0">E5-D5</f>
         <v>11.75</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G14" si="1">C5*9.8</f>
+        <f t="shared" ref="G5:G6" si="1">C5*9.8</f>
         <v>83.251000000000019</v>
       </c>
       <c r="H5">
         <v>-0.51900000000000002</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I14" si="2">G5/F5</f>
+        <f t="shared" ref="I5:I6" si="2">G5/F5</f>
         <v>7.0851914893617041</v>
       </c>
     </row>
@@ -1230,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,4 +1915,1296 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E4" s="1">
+        <f>D4-C4</f>
+        <v>-8.9499999999999993</v>
+      </c>
+      <c r="F4" s="1">
+        <f>B4*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="e">
+        <f>F4/D4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="2">
+        <v>-76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.54</v>
+      </c>
+      <c r="B5">
+        <f>A5</f>
+        <v>4.54</v>
+      </c>
+      <c r="C5">
+        <f>C4</f>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="D5" s="2">
+        <f>11.55+0.75</f>
+        <v>12.3</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E8" si="0">D5-C5</f>
+        <v>3.3500000000000014</v>
+      </c>
+      <c r="F5" s="1">
+        <f>B5*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H8" si="1">F5/E5</f>
+        <v>13.281194029850742</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B6">
+        <f>B5+A6</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C8" si="2">C5</f>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="D6" s="2">
+        <f>13.56+1.75</f>
+        <v>15.31</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3600000000000012</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:F8" si="3">B6*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>14.045125786163521</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:B8" si="4">B6+A7</f>
+        <v>13.75</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="D7" s="2">
+        <f>15.1+2.75</f>
+        <v>17.850000000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9000000000000021</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="3"/>
+        <v>134.75</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>15.140449438202243</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.548</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="4"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="D8" s="2">
+        <f>17.58+3.7</f>
+        <v>21.279999999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>12.329999999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>14.543422546634231</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="1">
+        <f>AVERAGE(H5:H8)</f>
+        <v>14.252547950212684</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <v>11.95</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12-C12</f>
+        <v>-11.95</v>
+      </c>
+      <c r="F12" s="1">
+        <f>B12*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="e">
+        <f>F12/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="2">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.54</v>
+      </c>
+      <c r="B13">
+        <f>A13</f>
+        <v>4.54</v>
+      </c>
+      <c r="C13">
+        <f>C12</f>
+        <v>11.95</v>
+      </c>
+      <c r="D13" s="2">
+        <f>17+0.75</f>
+        <v>17.75</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" ref="E13:E15" si="5">D13-C13</f>
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="F13" s="1">
+        <f>B13*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" ref="H13:H15" si="6">F13/E13</f>
+        <v>7.6710344827586203</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B14">
+        <f>B13+A14</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C15" si="7">C13</f>
+        <v>11.95</v>
+      </c>
+      <c r="D14" s="2">
+        <f>21.9+1.75</f>
+        <v>23.65</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="5"/>
+        <v>11.7</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" ref="F14:F15" si="8">B14*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="6"/>
+        <v>7.6347863247863259</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15" si="9">B14+A15</f>
+        <v>13.75</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="7"/>
+        <v>11.95</v>
+      </c>
+      <c r="D15" s="2">
+        <f>27.49+2.75</f>
+        <v>30.24</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="5"/>
+        <v>18.29</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="8"/>
+        <v>134.75</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="6"/>
+        <v>7.367413887370148</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1">
+        <f>AVERAGE(H13:H15)</f>
+        <v>7.5577448983050317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>16.05</v>
+      </c>
+      <c r="E21" s="1">
+        <f>D21-C21</f>
+        <v>-16.05</v>
+      </c>
+      <c r="F21" s="1">
+        <f>B21*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="e">
+        <f>F21/D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4.54</v>
+      </c>
+      <c r="B22">
+        <f>A22</f>
+        <v>4.54</v>
+      </c>
+      <c r="C22">
+        <f>C21</f>
+        <v>16.05</v>
+      </c>
+      <c r="D22" s="2">
+        <v>24.95</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" ref="E22:E23" si="10">D22-C22</f>
+        <v>8.8999999999999986</v>
+      </c>
+      <c r="F22" s="1">
+        <f>B22*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" ref="H22:H23" si="11">F22/E22</f>
+        <v>4.9991011235955067</v>
+      </c>
+      <c r="J22" s="2">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B23">
+        <f>B22+A23</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23" si="12">C22</f>
+        <v>16.05</v>
+      </c>
+      <c r="D23" s="2">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="10"/>
+        <v>19.150000000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23" si="13">B23*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="11"/>
+        <v>4.6645953002610971</v>
+      </c>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="1">
+        <f>AVERAGE(H22:H23)</f>
+        <v>4.8318482119283015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="E27" s="1">
+        <f>D27-C27</f>
+        <v>-8.9</v>
+      </c>
+      <c r="F27" s="1">
+        <f>B27*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="e">
+        <f>F27/D27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4.54</v>
+      </c>
+      <c r="B28">
+        <f>A28</f>
+        <v>4.54</v>
+      </c>
+      <c r="C28">
+        <f>C27</f>
+        <v>8.9</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" ref="E28:E31" si="14">D28-C28</f>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="F28" s="1">
+        <f>B28*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" ref="H28:H31" si="15">F28/E28</f>
+        <v>27.807500000000008</v>
+      </c>
+      <c r="J28" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B29">
+        <f>B28+A29</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C31" si="16">C28</f>
+        <v>8.9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>12.4</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="14"/>
+        <v>3.5</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" ref="F29:F31" si="17">B29*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="15"/>
+        <v>25.522000000000002</v>
+      </c>
+      <c r="J29" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:B31" si="18">B29+A30</f>
+        <v>13.75</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="16"/>
+        <v>8.9</v>
+      </c>
+      <c r="D30" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="14"/>
+        <v>5.6</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="17"/>
+        <v>134.75</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="15"/>
+        <v>24.0625</v>
+      </c>
+      <c r="J30" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4.548</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="18"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="16"/>
+        <v>8.9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>16.46</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="14"/>
+        <v>7.5600000000000005</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="17"/>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="15"/>
+        <v>23.719629629629633</v>
+      </c>
+      <c r="J31" s="2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="1">
+        <f>AVERAGE(H28:H31)</f>
+        <v>25.277907407407412</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <f>H32</f>
+        <v>25.277907407407412</v>
+      </c>
+      <c r="E36">
+        <f>D36/0.0254</f>
+        <v>995.19320501603988</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <f>H59</f>
+        <v>14.774528973201786</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ref="E37:E40" si="19">D37/0.0254</f>
+        <v>581.67436902369241</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <f>H67</f>
+        <v>7.457259050696365</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="19"/>
+        <v>293.5928760116679</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <f>H24</f>
+        <v>4.8318482119283015</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="19"/>
+        <v>190.23024456410636</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <f>H75</f>
+        <v>9.7746968597252426</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="19"/>
+        <v>384.83058502855289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <v>1.97</v>
+      </c>
+      <c r="E54" s="1">
+        <f>D54-C54</f>
+        <v>-1.97</v>
+      </c>
+      <c r="F54" s="1">
+        <f>B54*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="e">
+        <f>F54/D54</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>4.54</v>
+      </c>
+      <c r="B55">
+        <f>A55</f>
+        <v>4.54</v>
+      </c>
+      <c r="C55">
+        <f>C54</f>
+        <v>1.97</v>
+      </c>
+      <c r="D55" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" ref="E55:E58" si="20">D55-C55</f>
+        <v>2.9300000000000006</v>
+      </c>
+      <c r="F55" s="1">
+        <f>B55*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" ref="H55:H58" si="21">F55/E55</f>
+        <v>15.184982935153583</v>
+      </c>
+      <c r="J55" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B56">
+        <f>B55+A56</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ref="C56:C58" si="22">C55</f>
+        <v>1.97</v>
+      </c>
+      <c r="D56" s="2">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="20"/>
+        <v>6.03</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" ref="F56:F58" si="23">B56*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="21"/>
+        <v>14.813764510779437</v>
+      </c>
+      <c r="J56" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ref="B57:B58" si="24">B56+A57</f>
+        <v>13.75</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="22"/>
+        <v>1.97</v>
+      </c>
+      <c r="D57" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="20"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="23"/>
+        <v>134.75</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="21"/>
+        <v>14.520474137931036</v>
+      </c>
+      <c r="J57" s="2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>4.548</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="24"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="22"/>
+        <v>1.97</v>
+      </c>
+      <c r="D58" s="2">
+        <v>14.27</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="20"/>
+        <v>12.299999999999999</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="23"/>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="21"/>
+        <v>14.578894308943093</v>
+      </c>
+      <c r="J58" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="1">
+        <f>AVERAGE(H55:H58)</f>
+        <v>14.774528973201786</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C62" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E62" s="1">
+        <f>D62-C62</f>
+        <v>-5.5</v>
+      </c>
+      <c r="F62" s="1">
+        <f>B62*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="e">
+        <f>F62/D62</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J62" s="2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>4.54</v>
+      </c>
+      <c r="B63">
+        <f>A63</f>
+        <v>4.54</v>
+      </c>
+      <c r="C63">
+        <f>C62</f>
+        <v>5.5</v>
+      </c>
+      <c r="D63" s="2">
+        <v>11.48</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" ref="E63:E65" si="25">D63-C63</f>
+        <v>5.98</v>
+      </c>
+      <c r="F63" s="1">
+        <f>B63*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" ref="H63:H65" si="26">F63/E63</f>
+        <v>7.4401337792642144</v>
+      </c>
+      <c r="J63" s="2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B64">
+        <f>B63+A64</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ref="C64:C66" si="27">C63</f>
+        <v>5.5</v>
+      </c>
+      <c r="D64" s="2">
+        <v>17.18</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="25"/>
+        <v>11.68</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" ref="F64:F65" si="28">B64*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="26"/>
+        <v>7.6478595890410972</v>
+      </c>
+      <c r="J64" s="2">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B65">
+        <f t="shared" ref="B65:B66" si="29">B64+A65</f>
+        <v>13.75</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="27"/>
+        <v>5.5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>24</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="25"/>
+        <v>18.5</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="28"/>
+        <v>134.75</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="26"/>
+        <v>7.2837837837837842</v>
+      </c>
+      <c r="J65" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>4.548</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="29"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="27"/>
+        <v>5.5</v>
+      </c>
+      <c r="D66" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" ref="E66" si="30">D66-C66</f>
+        <v>25.7</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" ref="F66" si="31">B66*9.8</f>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" ref="H66" si="32">F66/E66</f>
+        <v>6.9774474708171219</v>
+      </c>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H67" s="1">
+        <f>AVERAGE(H63:H65)</f>
+        <v>7.457259050696365</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C70" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="E70" s="1">
+        <f>D70-C70</f>
+        <v>-4.95</v>
+      </c>
+      <c r="F70" s="1">
+        <f>B70*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="H70" s="1" t="e">
+        <f>F70/D70</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J70" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>4.54</v>
+      </c>
+      <c r="B71">
+        <f>A71</f>
+        <v>4.54</v>
+      </c>
+      <c r="C71">
+        <f>C70</f>
+        <v>4.95</v>
+      </c>
+      <c r="D71" s="2">
+        <v>9.48</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" ref="E71:E74" si="33">D71-C71</f>
+        <v>4.53</v>
+      </c>
+      <c r="F71" s="1">
+        <f>B71*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" ref="H71:H74" si="34">F71/E71</f>
+        <v>9.8216335540838848</v>
+      </c>
+      <c r="J71" s="2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="B72">
+        <f>B71+A72</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ref="C72:C74" si="35">C71</f>
+        <v>4.95</v>
+      </c>
+      <c r="D72" s="2">
+        <v>14.4</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="33"/>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" ref="F72:F74" si="36">B72*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="34"/>
+        <v>9.4525925925925947</v>
+      </c>
+      <c r="J72" s="2">
+        <v>369</v>
+      </c>
+      <c r="K72">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="B73">
+        <f t="shared" ref="B73:B74" si="37">B72+A73</f>
+        <v>13.75</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="35"/>
+        <v>4.95</v>
+      </c>
+      <c r="D73" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="33"/>
+        <v>13.55</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="36"/>
+        <v>134.75</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="34"/>
+        <v>9.9446494464944646</v>
+      </c>
+      <c r="J73" s="2">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>4.548</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="37"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="35"/>
+        <v>4.95</v>
+      </c>
+      <c r="D74" s="2">
+        <v>23.1</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="33"/>
+        <v>18.150000000000002</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="36"/>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="34"/>
+        <v>9.8799118457300281</v>
+      </c>
+      <c r="J74" s="2">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="1">
+        <f>AVERAGE(H71:H74)</f>
+        <v>9.7746968597252426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding more damping resolution
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="29">
   <si>
     <t>Mass</t>
   </si>
@@ -90,17 +90,29 @@
     <t>Inches to meters</t>
   </si>
   <si>
-    <t>Torque</t>
+    <t>Real Spring Constant</t>
   </si>
   <si>
-    <t>Real Spring Constant</t>
+    <t>K</t>
+  </si>
+  <si>
+    <t>StiffnessNew</t>
+  </si>
+  <si>
+    <t>Stiffness if 64</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>damping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +123,13 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -144,15 +163,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,11 +484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80583424"/>
-        <c:axId val="80584000"/>
+        <c:axId val="55777472"/>
+        <c:axId val="55778048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80583424"/>
+        <c:axId val="55777472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,12 +498,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80584000"/>
+        <c:crossAx val="55778048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80584000"/>
+        <c:axId val="55778048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80583424"/>
+        <c:crossAx val="55777472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -515,19 +603,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25.277907407407412</c:v>
+                  <c:v>995.19320501603988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.774528973201786</c:v>
+                  <c:v>581.67436902369241</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.457259050696365</c:v>
+                  <c:v>293.5928760116679</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8318482119283015</c:v>
+                  <c:v>190.23024456410639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7746968597252426</c:v>
+                  <c:v>384.83058502855283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,11 +630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125093568"/>
-        <c:axId val="125094144"/>
+        <c:axId val="122619008"/>
+        <c:axId val="122619584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125093568"/>
+        <c:axId val="122619008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,12 +644,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125094144"/>
+        <c:crossAx val="122619584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125094144"/>
+        <c:axId val="122619584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +660,173 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125093568"/>
+        <c:crossAx val="122619008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.23261679790026246"/>
+                  <c:y val="-1.7965879265091862E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5036526684164485E-2"/>
+                  <c:y val="2.1372849227179937E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3rd run'!$A$36:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3rd run'!$E$36:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>995.19320501603988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>581.67436902369241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>293.5928760116679</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>190.23024456410639</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384.83058502855283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="122621312"/>
+        <c:axId val="122621888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="122621312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="122621888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="122621888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="122621312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -633,16 +887,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -656,6 +910,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1931,7 +2215,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,8 +2601,8 @@
         <v>16.05</v>
       </c>
       <c r="E21" s="1">
-        <f>D21-C21</f>
-        <v>-16.05</v>
+        <f>(D21-C21)*$E$43</f>
+        <v>-0.40766999999999998</v>
       </c>
       <c r="F21" s="1">
         <f>B21*9.8</f>
@@ -2348,8 +2632,8 @@
         <v>24.95</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ref="E22:E23" si="10">D22-C22</f>
-        <v>8.8999999999999986</v>
+        <f t="shared" ref="E22:E23" si="10">(D22-C22)*$E$43</f>
+        <v>0.22605999999999996</v>
       </c>
       <c r="F22" s="1">
         <f>B22*9.8</f>
@@ -2357,7 +2641,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" ref="H22:H23" si="11">F22/E22</f>
-        <v>4.9991011235955067</v>
+        <v>196.81500486596485</v>
       </c>
       <c r="J22" s="2">
         <v>520</v>
@@ -2380,7 +2664,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" si="10"/>
-        <v>19.150000000000002</v>
+        <v>0.48641000000000001</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" ref="F23" si="13">B23*9.8</f>
@@ -2388,7 +2672,7 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" si="11"/>
-        <v>4.6645953002610971</v>
+        <v>183.64548426224792</v>
       </c>
       <c r="J23" s="2"/>
     </row>
@@ -2398,7 +2682,7 @@
       </c>
       <c r="H24" s="1">
         <f>AVERAGE(H22:H23)</f>
-        <v>4.8318482119283015</v>
+        <v>190.23024456410639</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2435,8 +2719,8 @@
         <v>8.9</v>
       </c>
       <c r="E27" s="1">
-        <f>D27-C27</f>
-        <v>-8.9</v>
+        <f>(D27-C27)*$E$43</f>
+        <v>-0.22606000000000001</v>
       </c>
       <c r="F27" s="1">
         <f>B27*9.8</f>
@@ -2466,16 +2750,16 @@
         <v>10.5</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ref="E28:E31" si="14">D28-C28</f>
-        <v>1.5999999999999996</v>
+        <f>(D28-C28)*$E$43</f>
+        <v>4.0639999999999989E-2</v>
       </c>
       <c r="F28" s="1">
         <f>B28*9.8</f>
         <v>44.492000000000004</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" ref="H28:H31" si="15">F28/E28</f>
-        <v>27.807500000000008</v>
+        <f t="shared" ref="H28:H31" si="14">F28/E28</f>
+        <v>1094.7834645669295</v>
       </c>
       <c r="J28" s="2">
         <v>105</v>
@@ -2490,23 +2774,23 @@
         <v>9.1150000000000002</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:C31" si="16">C28</f>
+        <f t="shared" ref="C29:C31" si="15">C28</f>
         <v>8.9</v>
       </c>
       <c r="D29" s="2">
         <v>12.4</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="14"/>
-        <v>3.5</v>
+        <f t="shared" ref="E29:E31" si="16">(D29-C29)*$E$43</f>
+        <v>8.8899999999999993E-2</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ref="F29:F31" si="17">B29*9.8</f>
         <v>89.327000000000012</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="15"/>
-        <v>25.522000000000002</v>
+        <f t="shared" si="14"/>
+        <v>1004.8031496062995</v>
       </c>
       <c r="J29" s="2">
         <v>156</v>
@@ -2521,23 +2805,23 @@
         <v>13.75</v>
       </c>
       <c r="C30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.9</v>
       </c>
       <c r="D30" s="2">
         <v>14.5</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="14"/>
-        <v>5.6</v>
+        <f t="shared" si="16"/>
+        <v>0.14223999999999998</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="17"/>
         <v>134.75</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="15"/>
-        <v>24.0625</v>
+        <f t="shared" si="14"/>
+        <v>947.34251968503952</v>
       </c>
       <c r="J30" s="2">
         <v>210</v>
@@ -2552,23 +2836,23 @@
         <v>18.298000000000002</v>
       </c>
       <c r="C31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.9</v>
       </c>
       <c r="D31" s="2">
         <v>16.46</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="14"/>
-        <v>7.5600000000000005</v>
+        <f t="shared" si="16"/>
+        <v>0.192024</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="17"/>
         <v>179.32040000000003</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="15"/>
-        <v>23.719629629629633</v>
+        <f t="shared" si="14"/>
+        <v>933.84368620589112</v>
       </c>
       <c r="J31" s="2">
         <v>268</v>
@@ -2580,101 +2864,159 @@
       </c>
       <c r="H32" s="1">
         <f>AVERAGE(H28:H31)</f>
-        <v>25.277907407407412</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+        <v>995.19320501603988</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>B36*64/10</f>
+        <v>19.2</v>
+      </c>
+      <c r="B36">
+        <f>C36</f>
+        <v>3</v>
+      </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36">
         <f>H32</f>
-        <v>25.277907407407412</v>
+        <v>995.19320501603988</v>
       </c>
       <c r="E36">
-        <f>D36/0.0254</f>
+        <f>D36</f>
         <v>995.19320501603988</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" ref="A37:A40" si="19">B37*64/10</f>
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ref="B37:B40" si="20">C37</f>
+        <v>5</v>
+      </c>
       <c r="C37">
         <v>5</v>
       </c>
       <c r="D37">
         <f>H59</f>
-        <v>14.774528973201786</v>
+        <v>581.67436902369241</v>
       </c>
       <c r="E37">
-        <f t="shared" ref="E37:E40" si="19">D37/0.0254</f>
+        <f t="shared" ref="E37:E40" si="21">D37</f>
         <v>581.67436902369241</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="19"/>
+        <v>64</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38">
         <f>H67</f>
-        <v>7.457259050696365</v>
+        <v>293.5928760116679</v>
       </c>
       <c r="E38">
+        <f t="shared" si="21"/>
+        <v>293.5928760116679</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
         <f t="shared" si="19"/>
-        <v>293.5928760116679</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="20"/>
+        <v>15</v>
+      </c>
       <c r="C39">
         <v>15</v>
       </c>
       <c r="D39">
         <f>H24</f>
-        <v>4.8318482119283015</v>
+        <v>190.23024456410639</v>
       </c>
       <c r="E39">
+        <f t="shared" si="21"/>
+        <v>190.23024456410639</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <f t="shared" si="19"/>
-        <v>190.23024456410636</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+        <v>44.8</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
       <c r="C40">
         <v>7</v>
       </c>
       <c r="D40">
         <f>H75</f>
-        <v>9.7746968597252426</v>
+        <v>384.83058502855283</v>
       </c>
       <c r="E40">
-        <f t="shared" si="19"/>
-        <v>384.83058502855289</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="21"/>
+        <v>384.83058502855283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>22</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="4">
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46">
-        <v>500</v>
+      <c r="D45" s="6">
+        <v>70</v>
+      </c>
+      <c r="E45" s="7">
+        <f>(E46-960.65)/-9.2099</f>
+        <v>39.158948522785266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="9">
+        <f xml:space="preserve"> -9.2099*D45 + 960.65</f>
+        <v>315.95699999999999</v>
+      </c>
+      <c r="E46" s="10">
+        <v>600</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2716,8 +3058,8 @@
         <v>1.97</v>
       </c>
       <c r="E54" s="1">
-        <f>D54-C54</f>
-        <v>-1.97</v>
+        <f>(D54-C54)*$E$43</f>
+        <v>-5.0037999999999999E-2</v>
       </c>
       <c r="F54" s="1">
         <f>B54*9.8</f>
@@ -2747,16 +3089,16 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" ref="E55:E58" si="20">D55-C55</f>
-        <v>2.9300000000000006</v>
+        <f t="shared" ref="E55:E58" si="22">(D55-C55)*$E$43</f>
+        <v>7.4422000000000016E-2</v>
       </c>
       <c r="F55" s="1">
         <f>B55*9.8</f>
         <v>44.492000000000004</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" ref="H55:H58" si="21">F55/E55</f>
-        <v>15.184982935153583</v>
+        <f t="shared" ref="H55:H58" si="23">F55/E55</f>
+        <v>597.83397382494422</v>
       </c>
       <c r="J55" s="2">
         <v>175</v>
@@ -2771,23 +3113,23 @@
         <v>9.1150000000000002</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:C58" si="22">C55</f>
+        <f t="shared" ref="C56:C58" si="24">C55</f>
         <v>1.97</v>
       </c>
       <c r="D56" s="2">
         <v>8</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="20"/>
-        <v>6.03</v>
+        <f t="shared" si="22"/>
+        <v>0.15316199999999999</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" ref="F56:F58" si="23">B56*9.8</f>
+        <f t="shared" ref="F56:F58" si="25">B56*9.8</f>
         <v>89.327000000000012</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="21"/>
-        <v>14.813764510779437</v>
+        <f t="shared" si="23"/>
+        <v>583.21907522753702</v>
       </c>
       <c r="J56" s="2">
         <v>257</v>
@@ -2798,27 +3140,27 @@
         <v>4.6349999999999998</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B58" si="24">B56+A57</f>
+        <f t="shared" ref="B57:B58" si="26">B56+A57</f>
         <v>13.75</v>
       </c>
       <c r="C57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.97</v>
       </c>
       <c r="D57" s="2">
         <v>11.25</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="20"/>
-        <v>9.2799999999999994</v>
+        <f t="shared" si="22"/>
+        <v>0.23571199999999998</v>
       </c>
       <c r="F57" s="1">
+        <f t="shared" si="25"/>
+        <v>134.75</v>
+      </c>
+      <c r="H57" s="1">
         <f t="shared" si="23"/>
-        <v>134.75</v>
-      </c>
-      <c r="H57" s="1">
-        <f t="shared" si="21"/>
-        <v>14.520474137931036</v>
+        <v>571.67221015476514</v>
       </c>
       <c r="J57" s="2">
         <v>357</v>
@@ -2829,27 +3171,27 @@
         <v>4.548</v>
       </c>
       <c r="B58">
+        <f t="shared" si="26"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C58">
         <f t="shared" si="24"/>
-        <v>18.298000000000002</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="22"/>
         <v>1.97</v>
       </c>
       <c r="D58" s="2">
         <v>14.27</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="20"/>
-        <v>12.299999999999999</v>
+        <f t="shared" si="22"/>
+        <v>0.31241999999999998</v>
       </c>
       <c r="F58" s="1">
+        <f t="shared" si="25"/>
+        <v>179.32040000000003</v>
+      </c>
+      <c r="H58" s="1">
         <f t="shared" si="23"/>
-        <v>179.32040000000003</v>
-      </c>
-      <c r="H58" s="1">
-        <f t="shared" si="21"/>
-        <v>14.578894308943093</v>
+        <v>573.97221688752336</v>
       </c>
       <c r="J58" s="2">
         <v>440</v>
@@ -2861,7 +3203,7 @@
       </c>
       <c r="H59" s="1">
         <f>AVERAGE(H55:H58)</f>
-        <v>14.774528973201786</v>
+        <v>581.67436902369241</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2898,8 +3240,8 @@
         <v>5.5</v>
       </c>
       <c r="E62" s="1">
-        <f>D62-C62</f>
-        <v>-5.5</v>
+        <f t="shared" ref="E62:E66" si="27">(D62-C62)*$E$43</f>
+        <v>-0.13969999999999999</v>
       </c>
       <c r="F62" s="1">
         <f>B62*9.8</f>
@@ -2929,16 +3271,16 @@
         <v>11.48</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" ref="E63:E65" si="25">D63-C63</f>
-        <v>5.98</v>
+        <f t="shared" si="27"/>
+        <v>0.151892</v>
       </c>
       <c r="F63" s="1">
         <f>B63*9.8</f>
         <v>44.492000000000004</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" ref="H63:H65" si="26">F63/E63</f>
-        <v>7.4401337792642144</v>
+        <f t="shared" ref="H63:H65" si="28">F63/E63</f>
+        <v>292.91865272693758</v>
       </c>
       <c r="J63" s="2">
         <v>339</v>
@@ -2953,23 +3295,23 @@
         <v>9.1150000000000002</v>
       </c>
       <c r="C64">
-        <f t="shared" ref="C64:C66" si="27">C63</f>
+        <f t="shared" ref="C64:C66" si="29">C63</f>
         <v>5.5</v>
       </c>
       <c r="D64" s="2">
         <v>17.18</v>
       </c>
       <c r="E64" s="1">
-        <f t="shared" si="25"/>
-        <v>11.68</v>
+        <f t="shared" si="27"/>
+        <v>0.29667199999999999</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" ref="F64:F65" si="28">B64*9.8</f>
+        <f t="shared" ref="F64:F65" si="30">B64*9.8</f>
         <v>89.327000000000012</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="26"/>
-        <v>7.6478595890410972</v>
+        <f t="shared" si="28"/>
+        <v>301.09683421421641</v>
       </c>
       <c r="J64" s="2">
         <v>529</v>
@@ -2980,27 +3322,27 @@
         <v>4.6349999999999998</v>
       </c>
       <c r="B65">
-        <f t="shared" ref="B65:B66" si="29">B64+A65</f>
+        <f t="shared" ref="B65:B66" si="31">B64+A65</f>
         <v>13.75</v>
       </c>
       <c r="C65">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>5.5</v>
       </c>
       <c r="D65" s="2">
         <v>24</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="25"/>
-        <v>18.5</v>
+        <f t="shared" si="27"/>
+        <v>0.46989999999999998</v>
       </c>
       <c r="F65" s="1">
+        <f t="shared" si="30"/>
+        <v>134.75</v>
+      </c>
+      <c r="H65" s="1">
         <f t="shared" si="28"/>
-        <v>134.75</v>
-      </c>
-      <c r="H65" s="1">
-        <f t="shared" si="26"/>
-        <v>7.2837837837837842</v>
+        <v>286.76314109384975</v>
       </c>
       <c r="J65" s="2">
         <v>705</v>
@@ -3011,27 +3353,27 @@
         <v>4.548</v>
       </c>
       <c r="B66">
+        <f t="shared" si="31"/>
+        <v>18.298000000000002</v>
+      </c>
+      <c r="C66">
         <f t="shared" si="29"/>
-        <v>18.298000000000002</v>
-      </c>
-      <c r="C66">
-        <f t="shared" si="27"/>
         <v>5.5</v>
       </c>
       <c r="D66" s="2">
         <v>31.2</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" ref="E66" si="30">D66-C66</f>
-        <v>25.7</v>
+        <f t="shared" si="27"/>
+        <v>0.65277999999999992</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" ref="F66" si="31">B66*9.8</f>
+        <f t="shared" ref="F66" si="32">B66*9.8</f>
         <v>179.32040000000003</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" ref="H66" si="32">F66/E66</f>
-        <v>6.9774474708171219</v>
+        <f t="shared" ref="H66" si="33">F66/E66</f>
+        <v>274.7026563313828</v>
       </c>
       <c r="J66" s="2"/>
     </row>
@@ -3041,7 +3383,7 @@
       </c>
       <c r="H67" s="1">
         <f>AVERAGE(H63:H65)</f>
-        <v>7.457259050696365</v>
+        <v>293.5928760116679</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3078,8 +3420,8 @@
         <v>4.95</v>
       </c>
       <c r="E70" s="1">
-        <f>D70-C70</f>
-        <v>-4.95</v>
+        <f t="shared" ref="E70:E74" si="34">(D70-C70)*$E$43</f>
+        <v>-0.12573000000000001</v>
       </c>
       <c r="F70" s="1">
         <f>B70*9.8</f>
@@ -3109,16 +3451,16 @@
         <v>9.48</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" ref="E71:E74" si="33">D71-C71</f>
-        <v>4.53</v>
+        <f t="shared" si="34"/>
+        <v>0.115062</v>
       </c>
       <c r="F71" s="1">
         <f>B71*9.8</f>
         <v>44.492000000000004</v>
       </c>
       <c r="H71" s="1">
-        <f t="shared" ref="H71:H74" si="34">F71/E71</f>
-        <v>9.8216335540838848</v>
+        <f t="shared" ref="H71:H74" si="35">F71/E71</f>
+        <v>386.67848638125537</v>
       </c>
       <c r="J71" s="2">
         <v>246</v>
@@ -3133,23 +3475,23 @@
         <v>9.1150000000000002</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72:C74" si="35">C71</f>
+        <f t="shared" ref="C72:C74" si="36">C71</f>
         <v>4.95</v>
       </c>
       <c r="D72" s="2">
         <v>14.4</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="33"/>
-        <v>9.4499999999999993</v>
+        <f t="shared" si="34"/>
+        <v>0.24002999999999997</v>
       </c>
       <c r="F72" s="1">
-        <f t="shared" ref="F72:F74" si="36">B72*9.8</f>
+        <f t="shared" ref="F72:F74" si="37">B72*9.8</f>
         <v>89.327000000000012</v>
       </c>
       <c r="H72" s="1">
-        <f t="shared" si="34"/>
-        <v>9.4525925925925947</v>
+        <f t="shared" si="35"/>
+        <v>372.14931466899981</v>
       </c>
       <c r="J72" s="2">
         <v>369</v>
@@ -3163,27 +3505,27 @@
         <v>4.6349999999999998</v>
       </c>
       <c r="B73">
-        <f t="shared" ref="B73:B74" si="37">B72+A73</f>
+        <f t="shared" ref="B73:B74" si="38">B72+A73</f>
         <v>13.75</v>
       </c>
       <c r="C73">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>4.95</v>
       </c>
       <c r="D73" s="2">
         <v>18.5</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="33"/>
-        <v>13.55</v>
+        <f t="shared" si="34"/>
+        <v>0.34417000000000003</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>134.75</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="34"/>
-        <v>9.9446494464944646</v>
+        <f t="shared" si="35"/>
+        <v>391.52163175175053</v>
       </c>
       <c r="J73" s="2">
         <v>497</v>
@@ -3194,27 +3536,27 @@
         <v>4.548</v>
       </c>
       <c r="B74">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>18.298000000000002</v>
       </c>
       <c r="C74">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>4.95</v>
       </c>
       <c r="D74" s="2">
         <v>23.1</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="33"/>
-        <v>18.150000000000002</v>
+        <f t="shared" si="34"/>
+        <v>0.46101000000000003</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>179.32040000000003</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="34"/>
-        <v>9.8799118457300281</v>
+        <f t="shared" si="35"/>
+        <v>388.97290731220585</v>
       </c>
       <c r="J74" s="2">
         <v>633</v>
@@ -3226,7 +3568,7 @@
       </c>
       <c r="H75" s="1">
         <f>AVERAGE(H71:H74)</f>
-        <v>9.7746968597252426</v>
+        <v>384.83058502855283</v>
       </c>
     </row>
   </sheetData>
@@ -3238,12 +3580,47 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C7:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>400</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>600</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>800</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Adding more torque leeway
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" tabRatio="850" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="32">
   <si>
     <t>Mass</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Inch To Meters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2257,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J9"/>
+    <sheetView topLeftCell="L20" workbookViewId="0">
+      <selection activeCell="T56" sqref="T56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,11 +3048,11 @@
         <v>17</v>
       </c>
       <c r="D45" s="6">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="E45" s="7">
         <f>(E46-960.65)/-9.2099</f>
-        <v>39.158948522785266</v>
+        <v>126.02199806729716</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3058,18 +3061,18 @@
       </c>
       <c r="D46" s="9">
         <f xml:space="preserve"> -9.2099*D45 + 960.65</f>
-        <v>315.95699999999999</v>
+        <v>730.40250000000003</v>
       </c>
       <c r="E46" s="10">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>5</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <v>1.97</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4.54</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4.5750000000000002</v>
       </c>
@@ -3179,8 +3182,11 @@
       <c r="J56" s="2">
         <v>257</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4.6349999999999998</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4.548</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>19</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>581.67436902369241</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>10</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C62" s="2">
         <v>5.5</v>
       </c>
@@ -3300,7 +3306,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4.54</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4.5750000000000002</v>
       </c>
@@ -3628,7 +3634,7 @@
   <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:C8"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding more data points
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="35">
   <si>
     <t>Mass</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>BROKLEN PULLY</t>
   </si>
 </sst>
 </file>
@@ -954,6 +957,357 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5th run'!$C$123</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5th run'!$B$124:$B$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5th run'!$C$124:$C$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4920.3777786516875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2814.3877851458888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1826.9158040000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1406.7251690800001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1153.287168478261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>938.95946460176992</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>796.20658600000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>675.81158917197456</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>609.08392365097586</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>558.43378684210529</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>502.40184610000017</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>493.42379977464793</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="131931456"/>
+        <c:axId val="44835968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="131931456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44835968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44835968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131931456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5th run'!$B$127:$B$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5th run'!$C$127:$C$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1406.7251690800001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1153.287168478261</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>938.95946460176992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>796.20658600000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>675.81158917197456</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>609.08392365097586</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>558.43378684210529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>502.40184610000017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="57844288"/>
+        <c:axId val="131929728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="57844288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131929728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="131929728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57844288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1033,6 +1387,71 @@
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4377,10 +4796,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M63"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="B2:W135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4594,7 +5016,10 @@
         <f>MEDIAN(I8:I10)</f>
         <v>4920.3777786516875</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9">
+        <f>MAX(I8:I11)-MIN(I8:I11)</f>
+        <v>333.05093944540567</v>
+      </c>
       <c r="K12" s="24"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4796,7 +5221,10 @@
         <f>MEDIAN(I19:I21)</f>
         <v>2814.3877851458888</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="9">
+        <f>MAX(I19:I22)-MIN(I19:I22)</f>
+        <v>394.45547427999963</v>
+      </c>
       <c r="K23" s="24"/>
     </row>
     <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5000,7 +5428,10 @@
         <f>MEDIAN(I30:I32)</f>
         <v>1826.9158040000004</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="9">
+        <f>MAX(I30:I33)-MIN(I30:I33)</f>
+        <v>338.58228230227428</v>
+      </c>
       <c r="K34" s="24"/>
     </row>
     <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5099,7 +5530,7 @@
         <v>-64</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M39:M42" si="16">E40/(K40-$K$39)</f>
+        <f t="shared" ref="M40:M42" si="16">E40/(K40-$K$39)</f>
         <v>-0.11815789473684211</v>
       </c>
     </row>
@@ -5228,7 +5659,10 @@
         <f>MEDIAN(I40:I42)</f>
         <v>1406.7251690800001</v>
       </c>
-      <c r="J44" s="9"/>
+      <c r="J44" s="9">
+        <f>MAX(I40:I43)-MIN(I40:I43)</f>
+        <v>131.43556461538469</v>
+      </c>
       <c r="K44" s="24"/>
     </row>
     <row r="45" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5454,7 +5888,10 @@
         <f>MEDIAN(I49:I51)</f>
         <v>1153.287168478261</v>
       </c>
-      <c r="J53" s="9"/>
+      <c r="J53" s="9">
+        <f>MAX(I49:I52)-MIN(I49:I52)</f>
+        <v>65.880275174092503</v>
+      </c>
       <c r="K53" s="24"/>
     </row>
     <row r="55" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5596,10 +6033,12 @@
         <f t="shared" si="28"/>
         <v>3.7250000000000001</v>
       </c>
-      <c r="E61" s="28"/>
+      <c r="E61" s="28">
+        <v>9.375</v>
+      </c>
       <c r="F61" s="21">
         <f t="shared" si="29"/>
-        <v>-9.4614948907927585E-2</v>
+        <v>0.14350992250464184</v>
       </c>
       <c r="G61" s="21">
         <f t="shared" si="30"/>
@@ -5608,10 +6047,12 @@
       <c r="H61" s="23"/>
       <c r="I61" s="21">
         <f t="shared" si="27"/>
-        <v>-1424.1935503355705</v>
+        <v>938.95946460176992</v>
       </c>
       <c r="J61" s="23"/>
-      <c r="K61" s="27"/>
+      <c r="K61" s="27">
+        <v>200</v>
+      </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="22">
@@ -5625,10 +6066,12 @@
         <f t="shared" si="28"/>
         <v>3.7250000000000001</v>
       </c>
-      <c r="E62" s="28"/>
+      <c r="E62" s="28">
+        <v>11.26</v>
+      </c>
       <c r="F62" s="21">
         <f t="shared" si="29"/>
-        <v>-9.4614948907927585E-2</v>
+        <v>0.19138889664999581</v>
       </c>
       <c r="G62" s="21">
         <f t="shared" si="30"/>
@@ -5637,10 +6080,12 @@
       <c r="H62" s="23"/>
       <c r="I62" s="21">
         <f t="shared" si="27"/>
-        <v>-1894.4363662281883</v>
+        <v>936.53290832116795</v>
       </c>
       <c r="J62" s="23"/>
-      <c r="K62" s="27"/>
+      <c r="K62" s="27">
+        <v>255</v>
+      </c>
     </row>
     <row r="63" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="8"/>
@@ -5654,12 +6099,1568 @@
       </c>
       <c r="I63" s="29">
         <f>MEDIAN(I59:I61)</f>
-        <v>936.56802202396818</v>
-      </c>
-      <c r="J63" s="9"/>
+        <v>938.95946460176992</v>
+      </c>
+      <c r="J63" s="9">
+        <f>MAX(I59:I62)-MIN(I59:I62)</f>
+        <v>36.608474567720918</v>
+      </c>
       <c r="K63" s="24"/>
+    </row>
+    <row r="65" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B66" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="11">
+        <v>35</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="11"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="19"/>
+      <c r="N66" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O66" s="11">
+        <v>40</v>
+      </c>
+      <c r="P66" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="18"/>
+      <c r="S66" s="18"/>
+      <c r="T66" s="18"/>
+      <c r="U66" s="18"/>
+      <c r="V66" s="18"/>
+      <c r="W66" s="19"/>
+    </row>
+    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B67" s="20"/>
+      <c r="C67" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" s="25"/>
+      <c r="K67" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="N67" s="20"/>
+      <c r="O67" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P67" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q67" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="R67" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="S67" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T67" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="U67" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="V67" s="25"/>
+      <c r="W67" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B68" s="22"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="28">
+        <v>4</v>
+      </c>
+      <c r="E68" s="23"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="27">
+        <v>49</v>
+      </c>
+      <c r="N68" s="22"/>
+      <c r="O68" s="23"/>
+      <c r="P68" s="28">
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="21"/>
+      <c r="S68" s="21"/>
+      <c r="T68" s="21"/>
+      <c r="U68" s="21"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="27">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B69" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C69" s="23">
+        <f>B69</f>
+        <v>4.54</v>
+      </c>
+      <c r="D69" s="23">
+        <f>D68</f>
+        <v>4</v>
+      </c>
+      <c r="E69" s="28">
+        <v>6.2</v>
+      </c>
+      <c r="F69" s="21">
+        <f>(E69-D69)/$F$2</f>
+        <v>5.58799698248163E-2</v>
+      </c>
+      <c r="G69" s="21">
+        <f>C69*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H69" s="23"/>
+      <c r="I69" s="21">
+        <f t="shared" ref="I69:I72" si="32">G69/F69</f>
+        <v>796.20658600000002</v>
+      </c>
+      <c r="J69" s="23"/>
+      <c r="K69" s="27">
+        <v>110</v>
+      </c>
+      <c r="N69" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="O69" s="23">
+        <f>N69</f>
+        <v>4.54</v>
+      </c>
+      <c r="P69" s="23">
+        <f>P68</f>
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="Q69" s="28">
+        <v>5.23</v>
+      </c>
+      <c r="R69" s="21">
+        <f>(Q69-P69)/$F$2</f>
+        <v>6.8706962898240048E-2</v>
+      </c>
+      <c r="S69" s="21">
+        <f>O69*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="T69" s="23"/>
+      <c r="U69" s="21">
+        <f t="shared" ref="U69:U72" si="33">S69/R69</f>
+        <v>647.56173353049905</v>
+      </c>
+      <c r="V69" s="23"/>
+      <c r="W69" s="27">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B70" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C70" s="23">
+        <f>C69+B70</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D70" s="23">
+        <f t="shared" ref="D70:D72" si="34">D69</f>
+        <v>4</v>
+      </c>
+      <c r="E70" s="28">
+        <v>8.25</v>
+      </c>
+      <c r="F70" s="21">
+        <f t="shared" ref="F70:F72" si="35">(E70-D70)/$F$2</f>
+        <v>0.10794994170703148</v>
+      </c>
+      <c r="G70" s="21">
+        <f t="shared" ref="G70:G72" si="36">C70*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H70" s="23"/>
+      <c r="I70" s="21">
+        <f t="shared" si="32"/>
+        <v>827.48539357647064</v>
+      </c>
+      <c r="J70" s="23"/>
+      <c r="K70" s="27">
+        <v>168</v>
+      </c>
+      <c r="N70" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="O70" s="23">
+        <f>O69+N70</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="P70" s="23">
+        <f t="shared" ref="P70:P72" si="37">P69</f>
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="Q70" s="28">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="R70" s="21">
+        <f t="shared" ref="R70:R72" si="38">(Q70-P70)/$F$2</f>
+        <v>0.12699993142003704</v>
+      </c>
+      <c r="S70" s="21">
+        <f t="shared" ref="S70:S72" si="39">O70*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="T70" s="23"/>
+      <c r="U70" s="21">
+        <f t="shared" si="33"/>
+        <v>703.36258454000006</v>
+      </c>
+      <c r="V70" s="23"/>
+      <c r="W70" s="27">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B71" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C71" s="23">
+        <f t="shared" ref="C71:C72" si="40">C70+B71</f>
+        <v>13.75</v>
+      </c>
+      <c r="D71" s="23">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="E71" s="28">
+        <v>10.73</v>
+      </c>
+      <c r="F71" s="21">
+        <f t="shared" si="35"/>
+        <v>0.17094190769136985</v>
+      </c>
+      <c r="G71" s="21">
+        <f t="shared" si="36"/>
+        <v>134.75</v>
+      </c>
+      <c r="H71" s="23"/>
+      <c r="I71" s="21">
+        <f t="shared" si="32"/>
+        <v>788.27949108469534</v>
+      </c>
+      <c r="J71" s="23"/>
+      <c r="K71" s="27">
+        <v>238</v>
+      </c>
+      <c r="N71" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="O71" s="23">
+        <f t="shared" ref="O71:O72" si="41">O70+N71</f>
+        <v>13.75</v>
+      </c>
+      <c r="P71" s="23">
+        <f t="shared" si="37"/>
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="Q71" s="28">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="R71" s="21">
+        <f t="shared" si="38"/>
+        <v>0.19519889459259693</v>
+      </c>
+      <c r="S71" s="21">
+        <f t="shared" si="39"/>
+        <v>134.75</v>
+      </c>
+      <c r="T71" s="23"/>
+      <c r="U71" s="21">
+        <f t="shared" si="33"/>
+        <v>690.3215322055953</v>
+      </c>
+      <c r="V71" s="23"/>
+      <c r="W71" s="27">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B72" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C72" s="23">
+        <f t="shared" si="40"/>
+        <v>18.29</v>
+      </c>
+      <c r="D72" s="23">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="E72" s="28">
+        <v>12.73</v>
+      </c>
+      <c r="F72" s="21">
+        <f t="shared" si="35"/>
+        <v>0.22174188025938465</v>
+      </c>
+      <c r="G72" s="21">
+        <f t="shared" si="36"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H72" s="23"/>
+      <c r="I72" s="21">
+        <f t="shared" si="32"/>
+        <v>808.33625019473095</v>
+      </c>
+      <c r="J72" s="23"/>
+      <c r="K72" s="27"/>
+      <c r="N72" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="O72" s="23">
+        <f t="shared" si="41"/>
+        <v>18.29</v>
+      </c>
+      <c r="P72" s="23">
+        <f t="shared" si="37"/>
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>34</v>
+      </c>
+      <c r="R72" s="21" t="e">
+        <f>(#REF!-P72)/$F$2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S72" s="21">
+        <f t="shared" si="39"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="T72" s="23"/>
+      <c r="U72" s="21" t="e">
+        <f t="shared" si="33"/>
+        <v>#REF!</v>
+      </c>
+      <c r="V72" s="23"/>
+      <c r="W72" s="27"/>
+    </row>
+    <row r="73" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I73" s="29">
+        <f>MEDIAN(I69:I71)</f>
+        <v>796.20658600000002</v>
+      </c>
+      <c r="J73" s="9">
+        <f>MAX(I69:I72)-MIN(I69:I72)</f>
+        <v>39.205902491775305</v>
+      </c>
+      <c r="K73" s="24"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="9"/>
+      <c r="S73" s="9"/>
+      <c r="T73" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="U73" s="29">
+        <f>MEDIAN(U69:U71)</f>
+        <v>690.3215322055953</v>
+      </c>
+      <c r="V73" s="9" t="e">
+        <f>MAX(U69:U72)-MIN(U69:U72)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W73" s="24"/>
+    </row>
+    <row r="74" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B75" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="11">
+        <v>40</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="11"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="19"/>
+    </row>
+    <row r="76" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B76" s="20"/>
+      <c r="C76" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J76" s="25"/>
+      <c r="K76" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="E77" s="23"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="23"/>
+      <c r="K77" s="27"/>
+    </row>
+    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B78" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C78" s="23">
+        <f>B78</f>
+        <v>4.54</v>
+      </c>
+      <c r="D78" s="23">
+        <f>D77</f>
+        <v>1.4</v>
+      </c>
+      <c r="E78" s="28">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F78" s="21">
+        <f>(E78-D78)/$F$2</f>
+        <v>6.8579962966819993E-2</v>
+      </c>
+      <c r="G78" s="21">
+        <f>C78*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H78" s="23"/>
+      <c r="I78" s="21">
+        <f t="shared" ref="I78:I81" si="42">G78/F78</f>
+        <v>648.76092192592603</v>
+      </c>
+      <c r="J78" s="23"/>
+      <c r="K78" s="27"/>
+    </row>
+    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B79" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C79" s="23">
+        <f>C78+B79</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D79" s="23">
+        <f t="shared" ref="D79:D81" si="43">D78</f>
+        <v>1.4</v>
+      </c>
+      <c r="E79" s="28">
+        <v>6.53</v>
+      </c>
+      <c r="F79" s="21">
+        <f t="shared" ref="F79:F81" si="44">(E79-D79)/$F$2</f>
+        <v>0.13030192963695802</v>
+      </c>
+      <c r="G79" s="21">
+        <f t="shared" ref="G79:G81" si="45">C79*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H79" s="23"/>
+      <c r="I79" s="21">
+        <f t="shared" si="42"/>
+        <v>685.53858142300192</v>
+      </c>
+      <c r="J79" s="23"/>
+      <c r="K79" s="27"/>
+    </row>
+    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B80" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C80" s="23">
+        <f t="shared" ref="C80:C81" si="46">C79+B80</f>
+        <v>13.75</v>
+      </c>
+      <c r="D80" s="23">
+        <f t="shared" si="43"/>
+        <v>1.4</v>
+      </c>
+      <c r="E80" s="28">
+        <v>9.25</v>
+      </c>
+      <c r="F80" s="21">
+        <f t="shared" si="44"/>
+        <v>0.19938989232945814</v>
+      </c>
+      <c r="G80" s="21">
+        <f t="shared" si="45"/>
+        <v>134.75</v>
+      </c>
+      <c r="H80" s="23"/>
+      <c r="I80" s="21">
+        <f t="shared" si="42"/>
+        <v>675.81158917197456</v>
+      </c>
+      <c r="J80" s="23"/>
+      <c r="K80" s="27"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C81" s="23">
+        <f t="shared" si="46"/>
+        <v>18.29</v>
+      </c>
+      <c r="D81" s="23">
+        <f t="shared" si="43"/>
+        <v>1.4</v>
+      </c>
+      <c r="E81" s="28">
+        <v>11.574999999999999</v>
+      </c>
+      <c r="F81" s="21">
+        <f t="shared" si="44"/>
+        <v>0.25844486043977533</v>
+      </c>
+      <c r="G81" s="21">
+        <f t="shared" si="45"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H81" s="23"/>
+      <c r="I81" s="21">
+        <f t="shared" si="42"/>
+        <v>693.5405861621623</v>
+      </c>
+      <c r="J81" s="23"/>
+      <c r="K81" s="27"/>
+    </row>
+    <row r="82" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I82" s="29">
+        <f>MEDIAN(I78:I80)</f>
+        <v>675.81158917197456</v>
+      </c>
+      <c r="J82" s="9">
+        <f>MAX(I78:I81)-MIN(I78:I81)</f>
+        <v>44.779664236236272</v>
+      </c>
+      <c r="K82" s="24"/>
+    </row>
+    <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="11">
+        <v>45</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="19"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="20"/>
+      <c r="C86" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G86" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I86" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J86" s="25"/>
+      <c r="K86" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="22"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="28">
+        <v>1.52</v>
+      </c>
+      <c r="E87" s="23"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="27">
+        <v>-61</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C88" s="23">
+        <f>B88</f>
+        <v>4.54</v>
+      </c>
+      <c r="D88" s="23">
+        <f>D87</f>
+        <v>1.52</v>
+      </c>
+      <c r="E88" s="28">
+        <v>4.3</v>
+      </c>
+      <c r="F88" s="21">
+        <f>(E88-D88)/$F$2</f>
+        <v>7.0611961869540579E-2</v>
+      </c>
+      <c r="G88" s="21">
+        <f>C88*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H88" s="23"/>
+      <c r="I88" s="21">
+        <f t="shared" ref="I88:I90" si="47">G88/F88</f>
+        <v>630.09154287769798</v>
+      </c>
+      <c r="J88" s="23"/>
+      <c r="K88" s="27">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C89" s="23">
+        <f>C88+B89</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D89" s="23">
+        <f t="shared" ref="D89:D91" si="48">D88</f>
+        <v>1.52</v>
+      </c>
+      <c r="E89" s="28">
+        <v>7.3</v>
+      </c>
+      <c r="F89" s="21">
+        <f t="shared" ref="F89:F91" si="49">(E89-D89)/$F$2</f>
+        <v>0.14681192072156279</v>
+      </c>
+      <c r="G89" s="21">
+        <f t="shared" ref="G89:G91" si="50">C89*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H89" s="23"/>
+      <c r="I89" s="21">
+        <f t="shared" si="47"/>
+        <v>608.4451423356403</v>
+      </c>
+      <c r="J89" s="23"/>
+      <c r="K89" s="27">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C90" s="23">
+        <f t="shared" ref="C90:C91" si="51">C89+B90</f>
+        <v>13.75</v>
+      </c>
+      <c r="D90" s="23">
+        <f t="shared" si="48"/>
+        <v>1.52</v>
+      </c>
+      <c r="E90" s="28">
+        <v>10.23</v>
+      </c>
+      <c r="F90" s="21">
+        <f t="shared" si="49"/>
+        <v>0.22123388053370452</v>
+      </c>
+      <c r="G90" s="21">
+        <f t="shared" si="50"/>
+        <v>134.75</v>
+      </c>
+      <c r="H90" s="23"/>
+      <c r="I90" s="21">
+        <f t="shared" si="47"/>
+        <v>609.08392365097586</v>
+      </c>
+      <c r="J90" s="23"/>
+      <c r="K90" s="27">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C91" s="23">
+        <f t="shared" si="51"/>
+        <v>18.29</v>
+      </c>
+      <c r="D91" s="23">
+        <f t="shared" si="48"/>
+        <v>1.52</v>
+      </c>
+      <c r="E91" s="28"/>
+      <c r="F91" s="21">
+        <f t="shared" si="49"/>
+        <v>-3.8607979151691257E-2</v>
+      </c>
+      <c r="G91" s="21">
+        <f t="shared" si="50"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H91" s="23"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="23"/>
+      <c r="K91" s="27">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="8"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I92" s="29">
+        <f>MEDIAN(I88:I90)</f>
+        <v>609.08392365097586</v>
+      </c>
+      <c r="J92" s="9">
+        <f>MAX(I88:I91)-MIN(I88:I91)</f>
+        <v>21.646400542057677</v>
+      </c>
+      <c r="K92" s="24"/>
+    </row>
+    <row r="94" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="11">
+        <v>50</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="11"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="19"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="20"/>
+      <c r="C96" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I96" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J96" s="25"/>
+      <c r="K96" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B97" s="22"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="28">
+        <v>1.75</v>
+      </c>
+      <c r="E97" s="23"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
+      <c r="J97" s="23"/>
+      <c r="K97" s="27"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B98" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C98" s="23">
+        <f>B98</f>
+        <v>4.54</v>
+      </c>
+      <c r="D98" s="23">
+        <f>D97</f>
+        <v>1.75</v>
+      </c>
+      <c r="E98" s="28">
+        <v>4.75</v>
+      </c>
+      <c r="F98" s="21">
+        <f>(E98-D98)/$F$2</f>
+        <v>7.6199958852022215E-2</v>
+      </c>
+      <c r="G98" s="21">
+        <f>C98*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H98" s="23"/>
+      <c r="I98" s="21">
+        <f t="shared" ref="I98:I100" si="52">G98/F98</f>
+        <v>583.88482973333339</v>
+      </c>
+      <c r="J98" s="23"/>
+      <c r="K98" s="27"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B99" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C99" s="23">
+        <f>C98+B99</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D99" s="23">
+        <f t="shared" ref="D99:D101" si="53">D98</f>
+        <v>1.75</v>
+      </c>
+      <c r="E99" s="28">
+        <v>8.25</v>
+      </c>
+      <c r="F99" s="21">
+        <f t="shared" ref="F99:F101" si="54">(E99-D99)/$F$2</f>
+        <v>0.16509991084604814</v>
+      </c>
+      <c r="G99" s="21">
+        <f t="shared" ref="G99:G101" si="55">C99*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H99" s="23"/>
+      <c r="I99" s="21">
+        <f t="shared" si="52"/>
+        <v>541.0481419538462</v>
+      </c>
+      <c r="J99" s="23"/>
+      <c r="K99" s="27"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B100" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C100" s="23">
+        <f t="shared" ref="C100:C101" si="56">C99+B100</f>
+        <v>13.75</v>
+      </c>
+      <c r="D100" s="23">
+        <f t="shared" si="53"/>
+        <v>1.75</v>
+      </c>
+      <c r="E100" s="28">
+        <v>11.25</v>
+      </c>
+      <c r="F100" s="21">
+        <f t="shared" si="54"/>
+        <v>0.24129986969807035</v>
+      </c>
+      <c r="G100" s="21">
+        <f t="shared" si="55"/>
+        <v>134.75</v>
+      </c>
+      <c r="H100" s="23"/>
+      <c r="I100" s="21">
+        <f t="shared" si="52"/>
+        <v>558.43378684210529</v>
+      </c>
+      <c r="J100" s="23"/>
+      <c r="K100" s="27"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B101" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C101" s="23">
+        <f t="shared" si="56"/>
+        <v>18.29</v>
+      </c>
+      <c r="D101" s="23">
+        <f t="shared" si="53"/>
+        <v>1.75</v>
+      </c>
+      <c r="E101" s="28"/>
+      <c r="F101" s="21">
+        <f t="shared" si="54"/>
+        <v>-4.4449975997012961E-2</v>
+      </c>
+      <c r="G101" s="21">
+        <f t="shared" si="55"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H101" s="23"/>
+      <c r="I101" s="21"/>
+      <c r="J101" s="23"/>
+      <c r="K101" s="27"/>
+    </row>
+    <row r="102" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="8"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I102" s="29">
+        <f>MEDIAN(I98:I100)</f>
+        <v>558.43378684210529</v>
+      </c>
+      <c r="J102" s="9">
+        <f>MAX(I98:I101)-MIN(I98:I101)</f>
+        <v>42.836687779487193</v>
+      </c>
+      <c r="K102" s="24"/>
+    </row>
+    <row r="104" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B105" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="11">
+        <v>55</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E105" s="11"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="19"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B106" s="20"/>
+      <c r="C106" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E106" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25"/>
+      <c r="K106" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B107" s="22"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="E107" s="23"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="23"/>
+      <c r="K107" s="27"/>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B108" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C108" s="23">
+        <f>B108</f>
+        <v>4.54</v>
+      </c>
+      <c r="D108" s="23">
+        <f>D107</f>
+        <v>1.2</v>
+      </c>
+      <c r="E108" s="28">
+        <v>4.7</v>
+      </c>
+      <c r="F108" s="21">
+        <f>(E108-D108)/$F$2</f>
+        <v>8.8899951994025922E-2</v>
+      </c>
+      <c r="G108" s="21">
+        <f>C108*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H108" s="23"/>
+      <c r="I108" s="21">
+        <f t="shared" ref="I108:I110" si="57">G108/F108</f>
+        <v>500.47271120000005</v>
+      </c>
+      <c r="J108" s="23"/>
+      <c r="K108" s="27"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B109" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C109" s="23">
+        <f>C108+B109</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D109" s="23">
+        <f t="shared" ref="D109:D111" si="58">D108</f>
+        <v>1.2</v>
+      </c>
+      <c r="E109" s="28">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F109" s="21">
+        <f t="shared" ref="F109:F111" si="59">(E109-D109)/$F$2</f>
+        <v>0.17779990398805182</v>
+      </c>
+      <c r="G109" s="21">
+        <f t="shared" ref="G109:G111" si="60">C109*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H109" s="23"/>
+      <c r="I109" s="21">
+        <f t="shared" si="57"/>
+        <v>502.40184610000017</v>
+      </c>
+      <c r="J109" s="23"/>
+      <c r="K109" s="27"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B110" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C110" s="23">
+        <f t="shared" ref="C110:C111" si="61">C109+B110</f>
+        <v>13.75</v>
+      </c>
+      <c r="D110" s="23">
+        <f t="shared" si="58"/>
+        <v>1.2</v>
+      </c>
+      <c r="E110" s="28">
+        <v>11.7</v>
+      </c>
+      <c r="F110" s="21">
+        <f t="shared" si="59"/>
+        <v>0.26669985598207774</v>
+      </c>
+      <c r="G110" s="21">
+        <f t="shared" si="60"/>
+        <v>134.75</v>
+      </c>
+      <c r="H110" s="23"/>
+      <c r="I110" s="21">
+        <f t="shared" si="57"/>
+        <v>505.24961666666672</v>
+      </c>
+      <c r="J110" s="23"/>
+      <c r="K110" s="27"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B111" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C111" s="23">
+        <f t="shared" si="61"/>
+        <v>18.29</v>
+      </c>
+      <c r="D111" s="23">
+        <f t="shared" si="58"/>
+        <v>1.2</v>
+      </c>
+      <c r="E111" s="28"/>
+      <c r="F111" s="21">
+        <f t="shared" si="59"/>
+        <v>-3.0479983540808886E-2</v>
+      </c>
+      <c r="G111" s="21">
+        <f t="shared" si="60"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H111" s="23"/>
+      <c r="I111" s="21"/>
+      <c r="J111" s="23"/>
+      <c r="K111" s="27"/>
+    </row>
+    <row r="112" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="8"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I112" s="29">
+        <f>MEDIAN(I108:I110)</f>
+        <v>502.40184610000017</v>
+      </c>
+      <c r="J112" s="9">
+        <f>MAX(I108:I111)-MIN(I108:I111)</f>
+        <v>4.7769054666666761</v>
+      </c>
+      <c r="K112" s="24"/>
+    </row>
+    <row r="113" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B114" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" s="11">
+        <v>60</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E114" s="11"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="19"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B115" s="20"/>
+      <c r="C115" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H115" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I115" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="25"/>
+      <c r="K115" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B116" s="22"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="28">
+        <v>1.7</v>
+      </c>
+      <c r="E116" s="23"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="21"/>
+      <c r="H116" s="21"/>
+      <c r="I116" s="21"/>
+      <c r="J116" s="23"/>
+      <c r="K116" s="27"/>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B117" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C117" s="23">
+        <f>B117</f>
+        <v>4.54</v>
+      </c>
+      <c r="D117" s="23">
+        <f>D116</f>
+        <v>1.7</v>
+      </c>
+      <c r="E117" s="28">
+        <v>5.25</v>
+      </c>
+      <c r="F117" s="21">
+        <f>(E117-D117)/$F$2</f>
+        <v>9.016995130822629E-2</v>
+      </c>
+      <c r="G117" s="21">
+        <f>C117*9.8</f>
+        <v>44.492000000000004</v>
+      </c>
+      <c r="H117" s="23"/>
+      <c r="I117" s="21">
+        <f t="shared" ref="I117:I119" si="62">G117/F117</f>
+        <v>493.42379977464793</v>
+      </c>
+      <c r="J117" s="23"/>
+      <c r="K117" s="27"/>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B118" s="22">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="C118" s="23">
+        <f>C117+B118</f>
+        <v>9.1150000000000002</v>
+      </c>
+      <c r="D118" s="23">
+        <f t="shared" ref="D118:D120" si="63">D117</f>
+        <v>1.7</v>
+      </c>
+      <c r="E118" s="28">
+        <v>8.75</v>
+      </c>
+      <c r="F118" s="21">
+        <f t="shared" ref="F118:F120" si="64">(E118-D118)/$F$2</f>
+        <v>0.1790699033022522</v>
+      </c>
+      <c r="G118" s="21">
+        <f t="shared" ref="G118:G120" si="65">C118*9.8</f>
+        <v>89.327000000000012</v>
+      </c>
+      <c r="H118" s="23"/>
+      <c r="I118" s="21">
+        <f t="shared" si="62"/>
+        <v>498.83871243971646</v>
+      </c>
+      <c r="J118" s="23"/>
+      <c r="K118" s="27"/>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B119" s="22">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="C119" s="23">
+        <f t="shared" ref="C119:C120" si="66">C118+B119</f>
+        <v>13.75</v>
+      </c>
+      <c r="D119" s="23">
+        <f t="shared" si="63"/>
+        <v>1.7</v>
+      </c>
+      <c r="E119" s="28">
+        <v>12.625</v>
+      </c>
+      <c r="F119" s="21">
+        <f t="shared" si="64"/>
+        <v>0.27749485015278091</v>
+      </c>
+      <c r="G119" s="21">
+        <f t="shared" si="65"/>
+        <v>134.75</v>
+      </c>
+      <c r="H119" s="23"/>
+      <c r="I119" s="21">
+        <f t="shared" si="62"/>
+        <v>485.59459725400455</v>
+      </c>
+      <c r="J119" s="23"/>
+      <c r="K119" s="27"/>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B120" s="22">
+        <v>4.54</v>
+      </c>
+      <c r="C120" s="23">
+        <f t="shared" si="66"/>
+        <v>18.29</v>
+      </c>
+      <c r="D120" s="23">
+        <f t="shared" si="63"/>
+        <v>1.7</v>
+      </c>
+      <c r="E120" s="28"/>
+      <c r="F120" s="21">
+        <f t="shared" si="64"/>
+        <v>-4.3179976682812586E-2</v>
+      </c>
+      <c r="G120" s="21">
+        <f t="shared" si="65"/>
+        <v>179.24200000000002</v>
+      </c>
+      <c r="H120" s="23"/>
+      <c r="I120" s="21"/>
+      <c r="J120" s="23"/>
+      <c r="K120" s="27"/>
+    </row>
+    <row r="121" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="8"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I121" s="29">
+        <f>MEDIAN(I117:I119)</f>
+        <v>493.42379977464793</v>
+      </c>
+      <c r="J121" s="9">
+        <f>MAX(I117:I120)-MIN(I117:I120)</f>
+        <v>13.244115185711905</v>
+      </c>
+      <c r="K121" s="24"/>
+    </row>
+    <row r="123" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <f>C5</f>
+        <v>5</v>
+      </c>
+      <c r="C124">
+        <f>I12</f>
+        <v>4920.3777786516875</v>
+      </c>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <f>C16</f>
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <f>I23</f>
+        <v>2814.3877851458888</v>
+      </c>
+    </row>
+    <row r="126" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <f>C27</f>
+        <v>15</v>
+      </c>
+      <c r="C126">
+        <f>I34</f>
+        <v>1826.9158040000004</v>
+      </c>
+    </row>
+    <row r="127" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <f>C37</f>
+        <v>20</v>
+      </c>
+      <c r="C127">
+        <f>I44</f>
+        <v>1406.7251690800001</v>
+      </c>
+    </row>
+    <row r="128" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <f>C46</f>
+        <v>25</v>
+      </c>
+      <c r="C128">
+        <f>I53</f>
+        <v>1153.287168478261</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <f>C56</f>
+        <v>30</v>
+      </c>
+      <c r="C129">
+        <f>I63</f>
+        <v>938.95946460176992</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <f>C66</f>
+        <v>35</v>
+      </c>
+      <c r="C130">
+        <f>I73</f>
+        <v>796.20658600000002</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <f>C75</f>
+        <v>40</v>
+      </c>
+      <c r="C131">
+        <f>I82</f>
+        <v>675.81158917197456</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <f>C85</f>
+        <v>45</v>
+      </c>
+      <c r="C132">
+        <f>I92</f>
+        <v>609.08392365097586</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <f>C95</f>
+        <v>50</v>
+      </c>
+      <c r="C133">
+        <f>I102</f>
+        <v>558.43378684210529</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <f>C105</f>
+        <v>55</v>
+      </c>
+      <c r="C134">
+        <f>I112</f>
+        <v>502.40184610000017</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <f>C114</f>
+        <v>60</v>
+      </c>
+      <c r="C135">
+        <f>I121</f>
+        <v>493.42379977464793</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-changing longs to ints -updating extra measurements from 1/21
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="39">
   <si>
     <t>Mass</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>1/17/13 cd</t>
+  </si>
+  <si>
+    <t>1/21/14 N-D</t>
   </si>
 </sst>
 </file>
@@ -8688,15 +8691,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G29"/>
+  <dimension ref="B4:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -8806,7 +8811,7 @@
         <v>493.42379977464793</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>80</v>
       </c>
@@ -8814,7 +8819,7 @@
         <v>358.85846150000003</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>90</v>
       </c>
@@ -8822,7 +8827,7 @@
         <v>316.72364029850746</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>95</v>
       </c>
@@ -8830,8 +8835,8 @@
         <v>285.10524849015587</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>24</v>
       </c>
@@ -8848,8 +8853,14 @@
       <c r="G22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="22">
         <v>1000</v>
       </c>
@@ -8861,7 +8872,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="22">
         <v>800</v>
       </c>
@@ -8873,7 +8884,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="22">
         <v>700</v>
       </c>
@@ -8885,7 +8896,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="22">
         <v>600</v>
       </c>
@@ -8902,8 +8913,14 @@
       <c r="G26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>540</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="22">
         <v>500</v>
       </c>
@@ -8920,8 +8937,14 @@
       <c r="G27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>470</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="22">
         <v>400</v>
       </c>
@@ -8938,8 +8961,14 @@
       <c r="G28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>380</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8">
         <v>300</v>
       </c>
@@ -8955,6 +8984,12 @@
       </c>
       <c r="G29">
         <v>3</v>
+      </c>
+      <c r="I29">
+        <v>350</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added presets for 400 & 600
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" tabRatio="648" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" tabRatio="648" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -388,6 +388,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3136,10 +3139,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B4:E24"/>
+  <dimension ref="B4:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,8 +3213,8 @@
         <v>267.48839106833202</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
         <v>24</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="22">
         <v>800</v>
       </c>
@@ -3235,7 +3238,7 @@
       <c r="D19" s="23"/>
       <c r="E19" s="31"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="22">
         <v>700</v>
       </c>
@@ -3249,21 +3252,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="40">
         <v>600</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="41">
         <v>96.396062114383</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="42">
         <v>575</v>
       </c>
       <c r="E21" s="31">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="22">
         <v>500</v>
       </c>
@@ -3277,21 +3280,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="22">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="40">
         <v>400</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="41">
         <v>140.49086049197209</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="42">
         <v>530</v>
       </c>
       <c r="E23" s="31">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8">
         <v>300</v>
       </c>
@@ -3314,7 +3320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C12" sqref="B12:C13"/>
     </sheetView>
   </sheetViews>
@@ -10091,7 +10097,7 @@
   </sheetPr>
   <dimension ref="A2:X260"/>
   <sheetViews>
-    <sheetView topLeftCell="A228" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D259" sqref="D259"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-Updating measurements -Scaling coulomb for more resolution
</commit_message>
<xml_diff>
--- a/calibration/voltage-torque calibration.xlsx
+++ b/calibration/voltage-torque calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680" tabRatio="648"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="13395" windowHeight="7620" tabRatio="648" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,14 @@
     <sheet name="4th run" sheetId="7" r:id="rId7"/>
     <sheet name="5th run" sheetId="8" r:id="rId8"/>
     <sheet name="resol1 run" sheetId="11" r:id="rId9"/>
-    <sheet name="Damping 2" sheetId="10" r:id="rId10"/>
-    <sheet name="Damping" sheetId="9" r:id="rId11"/>
+    <sheet name="Damping" sheetId="9" r:id="rId10"/>
+    <sheet name="Damping 2" sheetId="10" r:id="rId11"/>
     <sheet name="SystemID" sheetId="12" r:id="rId12"/>
     <sheet name="sine precomputations" sheetId="13" r:id="rId13"/>
     <sheet name="Free Decay 2-24" sheetId="14" r:id="rId14"/>
     <sheet name="Sheet3" sheetId="15" r:id="rId15"/>
+    <sheet name="Ticks calibration" sheetId="16" r:id="rId16"/>
+    <sheet name="System ID EVCK" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="amplitude">'sine precomputations'!$E$1</definedName>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="89">
   <si>
     <t>Mass</t>
   </si>
@@ -217,6 +219,90 @@
   <si>
     <t>g</t>
   </si>
+  <si>
+    <t>Mass Force</t>
+  </si>
+  <si>
+    <t>Force apply to system</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 1</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 2</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 3</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 4</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 5</t>
+  </si>
+  <si>
+    <t>Positive Test Run for NS 6</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 1</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 2</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 3</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 4</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 5</t>
+  </si>
+  <si>
+    <t>Negative Test Run for NS 6</t>
+  </si>
+  <si>
+    <t>zero pos = 1700</t>
+  </si>
+  <si>
+    <t>First Run</t>
+  </si>
+  <si>
+    <t>Second experiment</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>mean position</t>
+  </si>
+  <si>
+    <t>zero pos = 1740</t>
+  </si>
+  <si>
+    <t>zero pos = 1680</t>
+  </si>
+  <si>
+    <t>moving down:</t>
+  </si>
+  <si>
+    <t>moving up:</t>
+  </si>
+  <si>
+    <t>Using real tank</t>
+  </si>
+  <si>
+    <t>duty</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>torque</t>
+  </si>
+  <si>
+    <t>36/quad35</t>
+  </si>
 </sst>
 </file>
 
@@ -266,13 +352,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +387,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -458,8 +557,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,11 +805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123317632"/>
-        <c:axId val="123318208"/>
+        <c:axId val="127250944"/>
+        <c:axId val="127251520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123317632"/>
+        <c:axId val="127250944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,12 +819,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123318208"/>
+        <c:crossAx val="127251520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123318208"/>
+        <c:axId val="127251520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123317632"/>
+        <c:crossAx val="127250944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -770,7 +871,166 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.29031539807524059"/>
+                  <c:y val="6.8636264216972789E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'resol1 run'!$C$255:$C$260</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>741.32694847161576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>568.37380568888898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>462.57185613079025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>360.69876130256415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>337.33637877333342</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>267.84151708336822</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'resol1 run'!$B$255:$B$260</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="134203072"/>
+        <c:axId val="134203648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="134203072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134203648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="134203648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134203072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -906,11 +1166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125466816"/>
-        <c:axId val="125467392"/>
+        <c:axId val="134205376"/>
+        <c:axId val="134205952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125466816"/>
+        <c:axId val="134205376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,12 +1180,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125467392"/>
+        <c:crossAx val="134205952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125467392"/>
+        <c:axId val="134205952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,13 +1196,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125466816"/>
+        <c:crossAx val="134205376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -957,7 +1218,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -990,6 +1251,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1075,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131318336"/>
-        <c:axId val="131318912"/>
+        <c:axId val="134208256"/>
+        <c:axId val="134208832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131318336"/>
+        <c:axId val="134208256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,12 +1351,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131318912"/>
+        <c:crossAx val="134208832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131318912"/>
+        <c:axId val="134208832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,13 +1367,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131318336"/>
+        <c:crossAx val="134208256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1126,7 +1389,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1236,11 +1499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131320640"/>
-        <c:axId val="131321216"/>
+        <c:axId val="133603904"/>
+        <c:axId val="133604480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131320640"/>
+        <c:axId val="133603904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,12 +1513,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131321216"/>
+        <c:crossAx val="133604480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131321216"/>
+        <c:axId val="133604480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,13 +1529,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131320640"/>
+        <c:crossAx val="133603904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1287,7 +1551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4334,11 +4598,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131096064"/>
-        <c:axId val="131322944"/>
+        <c:axId val="133709312"/>
+        <c:axId val="133606208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131096064"/>
+        <c:axId val="133709312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4347,7 +4611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131322944"/>
+        <c:crossAx val="133606208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4355,7 +4619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131322944"/>
+        <c:axId val="133606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4366,7 +4630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131096064"/>
+        <c:crossAx val="133709312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4484,28 +4748,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0779378496544634</c:v>
+                  <c:v>1.0779210779999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3153178338343028</c:v>
+                  <c:v>2.3152818110000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5622370910199335</c:v>
+                  <c:v>3.562181668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7996170751997722</c:v>
+                  <c:v>4.7995424</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0478990856719452</c:v>
+                  <c:v>6.0478049890000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3111713822960747</c:v>
+                  <c:v>7.3110576309999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5553651329086211</c:v>
+                  <c:v>8.5552320230000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.8022843900942522</c:v>
+                  <c:v>9.8021318799999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4520,11 +4784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45068800"/>
-        <c:axId val="45068224"/>
+        <c:axId val="127253824"/>
+        <c:axId val="128188416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45068800"/>
+        <c:axId val="127253824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4534,12 +4798,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45068224"/>
+        <c:crossAx val="128188416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45068224"/>
+        <c:axId val="128188416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4550,7 +4814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45068800"/>
+        <c:crossAx val="127253824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4573,6 +4837,191 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Force apply to system</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.34114391951006123"/>
+                  <c:y val="3.4544692330125401E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.19639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.51700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.81799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.4379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.738</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.3199999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43.363145788076267</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.140309397377109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143.30121763617345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>193.07838120524579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>243.29411010539866</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294.11286632070153</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344.16413319655641</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>394.32504143535277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="128190144"/>
+        <c:axId val="128190720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="128190144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128190720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="128190720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128190144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4680,11 +5129,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123320512"/>
-        <c:axId val="123321088"/>
+        <c:axId val="128192448"/>
+        <c:axId val="128193024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123320512"/>
+        <c:axId val="128192448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4694,12 +5143,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123321088"/>
+        <c:crossAx val="128193024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123321088"/>
+        <c:axId val="128193024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4710,7 +5159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123320512"/>
+        <c:crossAx val="128192448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4731,7 +5180,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4845,11 +5294,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125534784"/>
-        <c:axId val="125535360"/>
+        <c:axId val="128195328"/>
+        <c:axId val="128195904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125534784"/>
+        <c:axId val="128195328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4859,12 +5308,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125535360"/>
+        <c:crossAx val="128195904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125535360"/>
+        <c:axId val="128195904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4875,7 +5324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125534784"/>
+        <c:crossAx val="128195328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4896,7 +5345,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4911,6 +5360,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5070,11 +5520,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125537088"/>
-        <c:axId val="125537664"/>
+        <c:axId val="127681088"/>
+        <c:axId val="127681664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125537088"/>
+        <c:axId val="127681088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5084,12 +5534,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125537664"/>
+        <c:crossAx val="127681664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125537664"/>
+        <c:axId val="127681664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5100,13 +5550,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125537088"/>
+        <c:crossAx val="127681088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5121,7 +5572,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5263,11 +5714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125539392"/>
-        <c:axId val="125539968"/>
+        <c:axId val="127683392"/>
+        <c:axId val="127683968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125539392"/>
+        <c:axId val="127683392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5277,12 +5728,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125539968"/>
+        <c:crossAx val="127683968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125539968"/>
+        <c:axId val="127683968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5293,13 +5744,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125539392"/>
+        <c:crossAx val="127683392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5314,7 +5766,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5329,6 +5781,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5488,11 +5941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125460480"/>
-        <c:axId val="125541696"/>
+        <c:axId val="127685696"/>
+        <c:axId val="127686272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125460480"/>
+        <c:axId val="127685696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5502,12 +5955,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125541696"/>
+        <c:crossAx val="127686272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125541696"/>
+        <c:axId val="127686272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5518,13 +5971,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125460480"/>
+        <c:crossAx val="127685696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5539,7 +5993,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5554,6 +6008,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5689,11 +6144,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125462208"/>
-        <c:axId val="125462784"/>
+        <c:axId val="127688000"/>
+        <c:axId val="134201344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125462208"/>
+        <c:axId val="127688000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5703,12 +6158,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125462784"/>
+        <c:crossAx val="134201344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125462784"/>
+        <c:axId val="134201344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5719,170 +6174,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125462208"/>
+        <c:crossAx val="127688000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.29031539807524059"/>
-                  <c:y val="6.8636264216972789E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'resol1 run'!$C$255:$C$260</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>741.32694847161576</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>568.37380568888898</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>462.57185613079025</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>360.69876130256415</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>337.33637877333342</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>267.84151708336822</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'resol1 run'!$B$255:$B$260</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="125464512"/>
-        <c:axId val="125465088"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="125464512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125465088"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="125465088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125464512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5901,16 +6200,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5954,6 +6253,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6222,16 +6551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6610,44 +6939,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F13"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>59</v>
       </c>
       <c r="E2">
-        <f>0.0254*(6+7/8)/2/3.1415926</f>
-        <v>2.7792432411510009E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>2.7792000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>2.4858000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="46"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E4" s="47">
+      <c r="E3" s="46">
         <v>9.8066499999999994</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="46">
+        <v>9.8066499999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -6661,10 +6996,13 @@
         <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3.9550000000000001</v>
       </c>
@@ -6675,15 +7013,18 @@
         <v>-0.255</v>
       </c>
       <c r="E6">
-        <f>B6*$E$4*$E$2</f>
-        <v>1.0779378496544634</v>
+        <v>1.0779210779999999</v>
       </c>
       <c r="F6">
         <f>B6*$E$4</f>
         <v>38.785300749999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>E6/F2</f>
+        <v>43.363145788076267</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6+4.54</f>
         <v>8.495000000000001</v>
@@ -6695,15 +7036,18 @@
         <v>-0.57299999999999995</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E13" si="0">B7*$E$4*$E$2</f>
-        <v>2.3153178338343028</v>
+        <v>2.3152818110000002</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F13" si="1">B7*$E$4</f>
+        <f t="shared" ref="F7:F13" si="0">B7*$E$4</f>
         <v>83.307491750000011</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>E7/0.024858</f>
+        <v>93.140309397377109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>B7+4.575</f>
         <v>13.07</v>
@@ -6715,15 +7059,18 @@
         <v>-0.86699999999999999</v>
       </c>
       <c r="E8">
+        <v>3.562181668</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>3.5622370910199335</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
         <v>128.17291549999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" ref="G8:G13" si="1">E8/0.024858</f>
+        <v>143.30121763617345</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>B8+4.54</f>
         <v>17.61</v>
@@ -6735,15 +7082,18 @@
         <v>-1.161</v>
       </c>
       <c r="E9">
+        <v>4.7995424</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>4.7996170751997722</v>
-      </c>
-      <c r="F9">
+        <v>172.69510649999998</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="1"/>
-        <v>172.69510649999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>193.07838120524579</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>B9+4.58</f>
         <v>22.189999999999998</v>
@@ -6755,15 +7105,18 @@
         <v>-1.526</v>
       </c>
       <c r="E10">
+        <v>6.0478049890000003</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
-        <v>6.0478990856719452</v>
-      </c>
-      <c r="F10">
+        <v>217.60956349999998</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="1"/>
-        <v>217.60956349999998</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>243.29411010539866</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>B10+4.635</f>
         <v>26.824999999999996</v>
@@ -6775,15 +7128,18 @@
         <v>-1.79</v>
       </c>
       <c r="E11">
+        <v>7.3110576309999997</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>7.3111713822960747</v>
-      </c>
-      <c r="F11">
+        <v>263.06338624999995</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="1"/>
-        <v>263.06338624999995</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>294.11286632070153</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>B11+4.565</f>
         <v>31.389999999999997</v>
@@ -6795,15 +7151,18 @@
         <v>-2.08</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>8.5553651329086211</v>
+        <v>8.5552320230000003</v>
       </c>
       <c r="F12">
+        <f>B12*$E$4</f>
+        <v>307.83074349999993</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="1"/>
-        <v>307.83074349999993</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>344.16413319655641</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>B12+4.575</f>
         <v>35.964999999999996</v>
@@ -6815,12 +7174,67 @@
         <v>-2.4</v>
       </c>
       <c r="E13">
+        <v>9.8021318799999992</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="0"/>
-        <v>9.8022843900942522</v>
-      </c>
-      <c r="F13">
+        <v>352.69616724999992</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="1"/>
-        <v>352.69616724999992</v>
+        <v>394.32504143535277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f>2.13+2.31</f>
+        <v>4.4399999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f>B39/4096</f>
+        <v>1.0839843749999999E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f>13*0.027792</f>
+        <v>0.36129600000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43">
+        <v>1000</v>
+      </c>
+      <c r="F43">
+        <f>(F42-0.2224)/-4.0965</f>
+        <v>-3.3906017331868675E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44">
+        <f>B40*(B43-1900)</f>
+        <v>-0.97558593749999989</v>
+      </c>
+      <c r="F44">
+        <f>F43/B40</f>
+        <v>-31.279064637687863</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45">
+        <f>B44*-4.0965+0.2224</f>
+        <v>4.2188877929687498</v>
       </c>
     </row>
   </sheetData>
@@ -6832,251 +7246,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="B4:F33"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>800</v>
-      </c>
-      <c r="C4">
-        <f>36725*B4^-0.929</f>
-        <v>73.78892894358394</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>700</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C11" si="0">36725*B5^-0.929</f>
-        <v>83.534470730350066</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>600</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>96.396062114383</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>500</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>114.1875278011925</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>400</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>140.49086049197209</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>300</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>183.53384319809689</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>200</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>267.48839106833202</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>3100</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>20.964610152525239</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
-        <v>800</v>
-      </c>
-      <c r="C19" s="35">
-        <v>73.78892894358394</v>
-      </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="31"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="22">
-        <v>700</v>
-      </c>
-      <c r="C20" s="35">
-        <v>83.534470730350066</v>
-      </c>
-      <c r="D20" s="23">
-        <v>600</v>
-      </c>
-      <c r="E20" s="31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="40">
-        <v>600</v>
-      </c>
-      <c r="C21" s="41">
-        <v>96.396062114383</v>
-      </c>
-      <c r="D21" s="42">
-        <v>575</v>
-      </c>
-      <c r="E21" s="31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
-        <v>500</v>
-      </c>
-      <c r="C22" s="35">
-        <v>114.1875278011925</v>
-      </c>
-      <c r="D22" s="23">
-        <v>560</v>
-      </c>
-      <c r="E22" s="31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="40">
-        <v>400</v>
-      </c>
-      <c r="C23" s="41">
-        <v>140.49086049197209</v>
-      </c>
-      <c r="D23" s="42">
-        <v>530</v>
-      </c>
-      <c r="E23" s="31">
-        <v>40</v>
-      </c>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="8">
-        <v>300</v>
-      </c>
-      <c r="C24" s="36">
-        <v>183.53384319809689</v>
-      </c>
-      <c r="D24" s="9">
-        <v>500</v>
-      </c>
-      <c r="E24" s="24">
-        <v>40</v>
-      </c>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>1000</v>
-      </c>
-      <c r="D31" s="41">
-        <f>C31*0.245+430.5</f>
-        <v>675.5</v>
-      </c>
-      <c r="E31">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <v>1600</v>
-      </c>
-      <c r="D32" s="41">
-        <f t="shared" ref="D32:D33" si="1">C32*0.245+430.5</f>
-        <v>822.5</v>
-      </c>
-      <c r="E32">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <v>2000</v>
-      </c>
-      <c r="D33" s="41">
-        <f t="shared" si="1"/>
-        <v>920.5</v>
-      </c>
-      <c r="E33">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="B12:C13"/>
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7382,17 +7555,261 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F12"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="B4:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>800</v>
+      </c>
+      <c r="C4">
+        <f>36725*B4^-0.929</f>
+        <v>73.78892894358394</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>700</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C11" si="0">36725*B5^-0.929</f>
+        <v>83.534470730350066</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>600</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>96.396062114383</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>114.1875278011925</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>400</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>140.49086049197209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>183.53384319809689</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>267.48839106833202</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3100</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>20.964610152525239</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="22">
+        <v>800</v>
+      </c>
+      <c r="C19" s="35">
+        <v>73.78892894358394</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="22">
+        <v>700</v>
+      </c>
+      <c r="C20" s="35">
+        <v>83.534470730350066</v>
+      </c>
+      <c r="D20" s="23">
+        <v>600</v>
+      </c>
+      <c r="E20" s="31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="40">
+        <v>600</v>
+      </c>
+      <c r="C21" s="41">
+        <v>96.396062114383</v>
+      </c>
+      <c r="D21" s="42">
+        <v>575</v>
+      </c>
+      <c r="E21" s="31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="22">
+        <v>500</v>
+      </c>
+      <c r="C22" s="35">
+        <v>114.1875278011925</v>
+      </c>
+      <c r="D22" s="23">
+        <v>560</v>
+      </c>
+      <c r="E22" s="31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="40">
+        <v>400</v>
+      </c>
+      <c r="C23" s="41">
+        <v>140.49086049197209</v>
+      </c>
+      <c r="D23" s="42">
+        <v>530</v>
+      </c>
+      <c r="E23" s="31">
+        <v>40</v>
+      </c>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="8">
+        <v>300</v>
+      </c>
+      <c r="C24" s="36">
+        <v>183.53384319809689</v>
+      </c>
+      <c r="D24" s="9">
+        <v>500</v>
+      </c>
+      <c r="E24" s="24">
+        <v>40</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31" s="41">
+        <f>C31*0.245+430.5</f>
+        <v>675.5</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1600</v>
+      </c>
+      <c r="D32" s="41">
+        <f t="shared" ref="D32:D33" si="1">C32*0.245+430.5</f>
+        <v>822.5</v>
+      </c>
+      <c r="E32">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>2000</v>
+      </c>
+      <c r="D33" s="41">
+        <f t="shared" si="1"/>
+        <v>920.5</v>
+      </c>
+      <c r="E33">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:H47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -7496,8 +7913,256 @@
         <v>41695</v>
       </c>
     </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="4">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="H18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="H19">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="H20">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>220</v>
+      </c>
+      <c r="H21">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22">
+        <v>250</v>
+      </c>
+      <c r="H22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="49"/>
+      <c r="C34" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1720</v>
+      </c>
+      <c r="D37">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1730</v>
+      </c>
+      <c r="D38">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7506,7 +8171,7 @@
   <dimension ref="A1:G1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34432,7 +35097,7 @@
         <v>0.24868988716485482</v>
       </c>
       <c r="E966">
-        <f t="shared" ref="E966:E1029" si="75">D966*amplitude+zerotorque</f>
+        <f t="shared" ref="E966:E1005" si="75">D966*amplitude+zerotorque</f>
         <v>248689.88716485482</v>
       </c>
       <c r="F966">
@@ -35603,6 +36268,243 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>29850</v>
+      </c>
+      <c r="B2">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>635.10638297872345</v>
+      </c>
+      <c r="E2">
+        <f>B2/39.37</f>
+        <v>1.1938023876047752</v>
+      </c>
+      <c r="F2">
+        <f>A2/E2</f>
+        <v>25004.138297872341</v>
+      </c>
+      <c r="I2">
+        <f>F2/100</f>
+        <v>250.04138297872342</v>
+      </c>
+      <c r="K2">
+        <f>I2^2</f>
+        <v>62520.69320191264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>29802</v>
+      </c>
+      <c r="B4">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <f>A4/B4</f>
+        <v>634.08510638297878</v>
+      </c>
+      <c r="E4">
+        <f>B4/39.37</f>
+        <v>1.1938023876047752</v>
+      </c>
+      <c r="F4">
+        <f>A4/E4</f>
+        <v>24963.930638297872</v>
+      </c>
+      <c r="I4">
+        <f>F4/100</f>
+        <v>249.63930638297873</v>
+      </c>
+      <c r="K4">
+        <f>I4^2</f>
+        <v>62319.783291374726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>29823</v>
+      </c>
+      <c r="B6">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <f>A6/B6</f>
+        <v>634.531914893617</v>
+      </c>
+      <c r="E6">
+        <f>B6/39.37</f>
+        <v>1.1938023876047752</v>
+      </c>
+      <c r="F6">
+        <f>A6/E6</f>
+        <v>24981.521489361701</v>
+      </c>
+      <c r="I6">
+        <f>F6/100</f>
+        <v>249.81521489361702</v>
+      </c>
+      <c r="K6">
+        <f>I6^2</f>
+        <v>62407.641592344051</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>29820</v>
+      </c>
+      <c r="B8">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <f>A8/B8</f>
+        <v>634.468085106383</v>
+      </c>
+      <c r="E8">
+        <f>B8/39.37</f>
+        <v>1.1938023876047752</v>
+      </c>
+      <c r="F8">
+        <f>A8/E8</f>
+        <v>24979.008510638298</v>
+      </c>
+      <c r="I8">
+        <f>F8/100</f>
+        <v>249.79008510638297</v>
+      </c>
+      <c r="K8">
+        <f>I8^2</f>
+        <v>62395.08661745405</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="22">
+        <v>800</v>
+      </c>
+      <c r="C4" s="35">
+        <v>73.78892894358394</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="22">
+        <v>700</v>
+      </c>
+      <c r="C5" s="35">
+        <v>83.534470730350066</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="40">
+        <v>600</v>
+      </c>
+      <c r="C6" s="41">
+        <v>96.396062114383</v>
+      </c>
+      <c r="D6" s="42">
+        <v>32</v>
+      </c>
+      <c r="E6" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="22">
+        <v>500</v>
+      </c>
+      <c r="C7" s="35">
+        <v>114.1875278011925</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="40">
+        <v>400</v>
+      </c>
+      <c r="C8" s="41">
+        <v>140.49086049197209</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
+        <v>300</v>
+      </c>
+      <c r="C9" s="36">
+        <v>183.53384319809689</v>
+      </c>
+      <c r="D9" s="9">
+        <v>26</v>
+      </c>
+      <c r="E9" s="24">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -35731,7 +36633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:I6"/>
     </sheetView>
   </sheetViews>
@@ -37875,7 +38777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -38516,7 +39418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W189"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A184" workbookViewId="0">
       <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
@@ -42077,8 +42979,8 @@
   </sheetPr>
   <dimension ref="A2:X260"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K267" sqref="K267"/>
+    <sheetView topLeftCell="E103" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43330,6 +44232,17 @@
       <c r="K37" s="19"/>
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
+      <c r="O37">
+        <f>540*39.37</f>
+        <v>21259.8</v>
+      </c>
+      <c r="P37">
+        <f>210*210</f>
+        <v>44100</v>
+      </c>
+      <c r="R37">
+        <v>212</v>
+      </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="20"/>

</xml_diff>